<commit_message>
enhance the test to exclude some fields
</commit_message>
<xml_diff>
--- a/src/app/app-playloader/data/sample.04.xlsx
+++ b/src/app/app-playloader/data/sample.04.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeylam/repo/njs/njstool/src/app/app-playloader/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3FF86D-8656-0D4F-B5B3-17C8C87D71F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F93D920-50BB-9B44-9C14-4036E824C4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" xr2:uid="{EA9BDBA2-0CC1-8A42-AB5A-3B400F638747}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,7 +683,7 @@
       </c>
       <c r="D14" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd hh:mm:ss.000Z")</f>
-        <v>2024-04-04 00:06:14.490Z</v>
+        <v>2024-04-04 11:05:13.380Z</v>
       </c>
     </row>
   </sheetData>

</xml_diff>